<commit_message>
[FIX] data and column name
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_expense_ledger.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_expense_ledger.xlsx
@@ -97,10 +97,10 @@
     <t xml:space="preserve">Header Description</t>
   </si>
   <si>
-    <t xml:space="preserve">Document Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Document Journal</t>
+    <t xml:space="preserve">Doc Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doc Journal</t>
   </si>
   <si>
     <t xml:space="preserve">Document number</t>
@@ -395,8 +395,8 @@
   </sheetPr>
   <dimension ref="A1:AX12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O13" activeCellId="0" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -426,7 +426,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="29.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="25.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="25.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="24.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="23.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="19.58"/>
@@ -444,7 +444,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="1" width="19.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="19.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="4" width="15.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="4" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="22.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="25.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="17.36"/>

</xml_diff>

<commit_message>
[IMP] Adjust Expense Ledger Report
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_expense_ledger.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_expense_ledger.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
   <si>
     <t xml:space="preserve">Expense Ledger Report</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">Partner</t>
   </si>
   <si>
+    <t xml:space="preserve">Charge Type</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fiscal Year From</t>
   </si>
   <si>
@@ -59,9 +62,6 @@
   </si>
   <si>
     <t xml:space="preserve">Run Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Charge Type</t>
   </si>
   <si>
     <t xml:space="preserve">Account Name</t>
@@ -396,7 +396,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AX13"/>
+  <dimension ref="A1:AX14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -730,10 +730,8 @@
         <v>4</v>
       </c>
       <c r="B6" s="9"/>
-      <c r="C6" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="9"/>
+      <c r="C6" s="0"/>
+      <c r="D6" s="0"/>
       <c r="E6" s="0"/>
       <c r="F6" s="0"/>
       <c r="G6" s="0"/>
@@ -783,11 +781,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
+      <c r="D7" s="9"/>
       <c r="E7" s="0"/>
       <c r="F7" s="0"/>
       <c r="G7" s="0"/>
@@ -840,10 +840,8 @@
         <v>7</v>
       </c>
       <c r="B8" s="9"/>
-      <c r="C8" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11"/>
       <c r="E8" s="0"/>
       <c r="F8" s="0"/>
       <c r="G8" s="0"/>
@@ -893,13 +891,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="12"/>
+      <c r="D9" s="9"/>
       <c r="E9" s="0"/>
       <c r="F9" s="0"/>
       <c r="G9" s="0"/>
@@ -948,12 +946,14 @@
       <c r="AX9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="0"/>
-      <c r="D10" s="0"/>
+      <c r="D10" s="12"/>
       <c r="E10" s="0"/>
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
@@ -1005,7 +1005,7 @@
       <c r="A11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="12"/>
+      <c r="B11" s="9"/>
       <c r="C11" s="0"/>
       <c r="D11" s="0"/>
       <c r="E11" s="0"/>
@@ -1055,9 +1055,11 @@
       <c r="AW11" s="0"/>
       <c r="AX11" s="0"/>
     </row>
-    <row r="12" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0"/>
-      <c r="B12" s="0"/>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="12"/>
       <c r="C12" s="0"/>
       <c r="D12" s="0"/>
       <c r="E12" s="0"/>
@@ -1107,155 +1109,207 @@
       <c r="AW12" s="0"/>
       <c r="AX12" s="0"/>
     </row>
-    <row r="13" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="14" t="s">
+    <row r="13" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0"/>
+      <c r="B13" s="0"/>
+      <c r="C13" s="0"/>
+      <c r="D13" s="0"/>
+      <c r="E13" s="0"/>
+      <c r="F13" s="0"/>
+      <c r="G13" s="0"/>
+      <c r="H13" s="0"/>
+      <c r="I13" s="0"/>
+      <c r="J13" s="0"/>
+      <c r="K13" s="0"/>
+      <c r="L13" s="0"/>
+      <c r="M13" s="0"/>
+      <c r="N13" s="0"/>
+      <c r="O13" s="0"/>
+      <c r="P13" s="0"/>
+      <c r="Q13" s="0"/>
+      <c r="R13" s="0"/>
+      <c r="S13" s="0"/>
+      <c r="T13" s="0"/>
+      <c r="U13" s="0"/>
+      <c r="V13" s="0"/>
+      <c r="W13" s="0"/>
+      <c r="X13" s="0"/>
+      <c r="Y13" s="0"/>
+      <c r="Z13" s="0"/>
+      <c r="AA13" s="0"/>
+      <c r="AB13" s="0"/>
+      <c r="AC13" s="0"/>
+      <c r="AD13" s="0"/>
+      <c r="AE13" s="0"/>
+      <c r="AF13" s="0"/>
+      <c r="AG13" s="0"/>
+      <c r="AH13" s="0"/>
+      <c r="AI13" s="0"/>
+      <c r="AJ13" s="0"/>
+      <c r="AK13" s="0"/>
+      <c r="AL13" s="0"/>
+      <c r="AM13" s="0"/>
+      <c r="AN13" s="0"/>
+      <c r="AO13" s="0"/>
+      <c r="AP13" s="0"/>
+      <c r="AQ13" s="0"/>
+      <c r="AR13" s="0"/>
+      <c r="AS13" s="0"/>
+      <c r="AT13" s="0"/>
+      <c r="AU13" s="0"/>
+      <c r="AV13" s="0"/>
+      <c r="AW13" s="0"/>
+      <c r="AX13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C14" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D14" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E14" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F14" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="G14" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H14" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="14" t="s">
+      <c r="I14" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="14" t="s">
+      <c r="J14" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="K13" s="14" t="s">
+      <c r="K14" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="L13" s="14" t="s">
+      <c r="L14" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="M13" s="14" t="s">
+      <c r="M14" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="N13" s="14" t="s">
+      <c r="N14" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="O13" s="14" t="s">
+      <c r="O14" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="P13" s="14" t="s">
+      <c r="P14" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="Q13" s="14" t="s">
+      <c r="Q14" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="R13" s="14" t="s">
+      <c r="R14" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="S13" s="14" t="s">
+      <c r="S14" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="T13" s="14" t="s">
+      <c r="T14" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="U13" s="14" t="s">
+      <c r="U14" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="V13" s="14" t="s">
+      <c r="V14" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="W13" s="14" t="s">
+      <c r="W14" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="X13" s="14" t="s">
+      <c r="X14" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="Y13" s="14" t="s">
+      <c r="Y14" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="Z13" s="14" t="s">
+      <c r="Z14" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="AA13" s="14" t="s">
+      <c r="AA14" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="AB13" s="14" t="s">
+      <c r="AB14" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="AC13" s="14" t="s">
+      <c r="AC14" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="AD13" s="14" t="s">
+      <c r="AD14" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="AE13" s="14" t="s">
+      <c r="AE14" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="AF13" s="14" t="s">
+      <c r="AF14" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="AG13" s="14" t="s">
+      <c r="AG14" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="AH13" s="14" t="s">
+      <c r="AH14" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="AI13" s="14" t="s">
+      <c r="AI14" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AJ13" s="14" t="s">
+      <c r="AJ14" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="AK13" s="14" t="s">
+      <c r="AK14" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="AL13" s="14" t="s">
+      <c r="AL14" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="AM13" s="14" t="s">
+      <c r="AM14" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="AN13" s="14" t="s">
+      <c r="AN14" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="AO13" s="14" t="s">
+      <c r="AO14" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="AP13" s="14" t="s">
+      <c r="AP14" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="AQ13" s="14" t="s">
+      <c r="AQ14" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="AR13" s="14" t="s">
+      <c r="AR14" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="AS13" s="14" t="s">
+      <c r="AS14" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="AT13" s="14" t="s">
+      <c r="AT14" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="AU13" s="14" t="s">
+      <c r="AU14" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="AV13" s="14" t="s">
+      <c r="AV14" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="AW13" s="14" t="s">
+      <c r="AW14" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="AX13" s="14" t="s">
+      <c r="AX14" s="14" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>